<commit_message>
updating lending files to 1.0.1
Signed-off-by: mathurrohit875 <mathurrohit875@gmail.com>
</commit_message>
<xml_diff>
--- a/src/main/java/data/LendingData.xlsx
+++ b/src/main/java/data/LendingData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohit.mathur\ChainProject\ChainTestProject\src\main\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948397E7-EACC-454A-A573-AE576CF6390C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FEB2BA-992D-4FCB-9F56-39B2212D5926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="97">
   <si>
     <t>Type</t>
   </si>
@@ -298,9 +298,6 @@
     <t>Residence Stability</t>
   </si>
   <si>
-    <t>CSP182823</t>
-  </si>
-  <si>
     <t>Wallet exposure</t>
   </si>
   <si>
@@ -308,6 +305,21 @@
   </si>
   <si>
     <t>cussdvioy</t>
+  </si>
+  <si>
+    <t>CSP186606</t>
+  </si>
+  <si>
+    <t>CSP186625</t>
+  </si>
+  <si>
+    <t>CSP186834</t>
+  </si>
+  <si>
+    <t>CSP186912</t>
+  </si>
+  <si>
+    <t>CSP200048</t>
   </si>
 </sst>
 </file>
@@ -948,7 +960,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B35">
         <v>10000</v>
@@ -964,10 +976,10 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" t="s">
         <v>91</v>
-      </c>
-      <c r="B37" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
@@ -975,7 +987,7 @@
         <v>80</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -983,7 +995,7 @@
         <v>81</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -997,7 +1009,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:B19"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1140,7 +1152,7 @@
         <v>80</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -1156,7 +1168,7 @@
         <v>81</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -1209,7 +1221,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1351,7 +1363,7 @@
         <v>80</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -1367,7 +1379,7 @@
         <v>81</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -1411,7 +1423,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B26">
         <v>10000</v>
@@ -1434,7 +1446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEAA7BCB-65AD-4776-B743-29A58193C791}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -1721,12 +1733,12 @@
         <v>86</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B36">
         <v>10000</v>
@@ -1742,10 +1754,10 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" t="s">
         <v>91</v>
-      </c>
-      <c r="B38" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1758,7 +1770,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1900,7 +1912,7 @@
         <v>80</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -1916,7 +1928,7 @@
         <v>81</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -1944,7 +1956,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24">
         <v>10000</v>

</xml_diff>